<commit_message>
Gantt Chart for Development+SysArchi
*Ma'am Ria's Deliverables.
</commit_message>
<xml_diff>
--- a/forms/GanttChart.xlsx
+++ b/forms/GanttChart.xlsx
@@ -4,18 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="11340" windowHeight="5520" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="11340" windowHeight="5520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProgressSheet" sheetId="1" r:id="rId1"/>
     <sheet name="GanttChart" sheetId="4" r:id="rId2"/>
+    <sheet name="GanttChard(Dev-Summarized)" sheetId="6" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>Task at Hand</t>
   </si>
@@ -90,6 +94,60 @@
   </si>
   <si>
     <t>Time /Task</t>
+  </si>
+  <si>
+    <t>Time/Task</t>
+  </si>
+  <si>
+    <t>Create Sentiment  Analyzer  Module</t>
+  </si>
+  <si>
+    <t>Create Learner Module</t>
+  </si>
+  <si>
+    <t>Create Word Normalizer/Learner Module</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
   </si>
 </sst>
 </file>
@@ -113,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,8 +184,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -178,11 +242,114 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -192,18 +359,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47838</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2857500" y="1714500"/>
+          <a:ext cx="5810250" cy="4429338"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -495,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X25"/>
+  <dimension ref="A2:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,8 +1171,8 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4"/>
@@ -938,8 +1199,8 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4"/>
@@ -968,13 +1229,13 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -994,9 +1255,9 @@
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
+    <row r="7" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1022,8 +1283,8 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4"/>
@@ -1078,8 +1339,8 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="4"/>
@@ -1106,8 +1367,8 @@
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4"/>
@@ -1134,8 +1395,8 @@
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4"/>
@@ -1162,8 +1423,8 @@
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="4"/>
@@ -1190,8 +1451,8 @@
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="4"/>
@@ -1218,8 +1479,8 @@
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="4"/>
@@ -1246,8 +1507,8 @@
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="4"/>
@@ -1274,8 +1535,8 @@
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="4"/>
@@ -1330,8 +1591,8 @@
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="4"/>
@@ -1358,8 +1619,8 @@
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="4"/>
@@ -1414,8 +1675,8 @@
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="4"/>
@@ -1442,8 +1703,8 @@
       <c r="W22" s="4"/>
       <c r="X22" s="4"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="4"/>
@@ -1498,8 +1759,8 @@
       <c r="W24" s="8"/>
       <c r="X24" s="4"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="4"/>
@@ -1526,7 +1787,225 @@
       <c r="W25" s="4"/>
       <c r="X25" s="8"/>
     </row>
+    <row r="26" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="30" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="21"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42296</v>
+      </c>
+      <c r="C3" s="3">
+        <v>42303</v>
+      </c>
+      <c r="D3" s="5">
+        <v>42310</v>
+      </c>
+      <c r="E3" s="5">
+        <v>42317</v>
+      </c>
+      <c r="F3" s="5">
+        <v>42324</v>
+      </c>
+      <c r="G3" s="5">
+        <v>42331</v>
+      </c>
+      <c r="H3" s="3">
+        <v>42338</v>
+      </c>
+      <c r="I3" s="5">
+        <v>42345</v>
+      </c>
+      <c r="J3" s="5">
+        <v>42352</v>
+      </c>
+      <c r="K3" s="5">
+        <v>42359</v>
+      </c>
+      <c r="L3" s="5">
+        <v>42366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="J17" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Progress Sheet of Dev-Summarized
</commit_message>
<xml_diff>
--- a/forms/GanttChart.xlsx
+++ b/forms/GanttChart.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anj Lasala\Documents\GitHub\InappExp\forms\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="11340" windowHeight="5520" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="11340" windowHeight="5520" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ProgressSheet" sheetId="1" r:id="rId1"/>
     <sheet name="GanttChart" sheetId="4" r:id="rId2"/>
     <sheet name="GanttChard(Dev-Summarized)" sheetId="6" r:id="rId3"/>
+    <sheet name="Progress Sheet 2" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>Task at Hand</t>
   </si>
@@ -148,13 +154,49 @@
   </si>
   <si>
     <t>December</t>
+  </si>
+  <si>
+    <t>Thesis Title:</t>
+  </si>
+  <si>
+    <t>Inappropriate Expressions Recognition using Bootstrapping as Semi-Supervised Learning</t>
+  </si>
+  <si>
+    <t>Members:</t>
+  </si>
+  <si>
+    <t>Joshua S. Dapitan</t>
+  </si>
+  <si>
+    <t>Anjanette R. Lasala</t>
+  </si>
+  <si>
+    <t>Section:</t>
+  </si>
+  <si>
+    <t>BSCS 4-2</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Create Sentiment Analyzer Module</t>
+  </si>
+  <si>
+    <t>No. of Days Delayed</t>
+  </si>
+  <si>
+    <t>PROGRESS SHEET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +212,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +240,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -349,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -375,6 +431,35 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,6 +499,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -429,7 +517,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
+      <xdr:colOff>534458</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>47838</xdr:rowOff>
     </xdr:to>
@@ -510,7 +598,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -545,7 +633,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -754,45 +842,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="93.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="33" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>42296</v>
       </c>
@@ -802,8 +895,9 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>42303</v>
       </c>
@@ -813,8 +907,9 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>42310</v>
       </c>
@@ -824,8 +919,9 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>42317</v>
       </c>
@@ -835,8 +931,9 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>42324</v>
       </c>
@@ -846,8 +943,9 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>42331</v>
       </c>
@@ -857,8 +955,9 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>42338</v>
       </c>
@@ -868,8 +967,9 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>42345</v>
       </c>
@@ -879,8 +979,9 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>42352</v>
       </c>
@@ -890,8 +991,9 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>42359</v>
       </c>
@@ -901,8 +1003,9 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>42366</v>
       </c>
@@ -912,8 +1015,9 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>42373</v>
       </c>
@@ -923,8 +1027,9 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>42380</v>
       </c>
@@ -934,8 +1039,9 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>42387</v>
       </c>
@@ -945,8 +1051,9 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>42394</v>
       </c>
@@ -956,8 +1063,9 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>42401</v>
       </c>
@@ -967,8 +1075,9 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>42408</v>
       </c>
@@ -978,8 +1087,9 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>42415</v>
       </c>
@@ -989,8 +1099,9 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>42422</v>
       </c>
@@ -1000,8 +1111,9 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>42429</v>
       </c>
@@ -1011,8 +1123,9 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>42436</v>
       </c>
@@ -1022,8 +1135,9 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>42443</v>
       </c>
@@ -1033,8 +1147,9 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>42450</v>
       </c>
@@ -1044,6 +1159,7 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1055,18 +1171,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -1798,22 +1928,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="30" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="30" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2008,4 +2134,248 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="3">
+        <v>42296</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="3">
+        <v>42310</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="3">
+        <v>42324</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="3">
+        <v>42331</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="3">
+        <v>42359</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:K5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>